<commit_message>
small independent set improvements
</commit_message>
<xml_diff>
--- a/cplex-cpp/cplex float.xlsx
+++ b/cplex-cpp/cplex float.xlsx
@@ -12,14 +12,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="26083" windowHeight="11045"/>
   </bookViews>
   <sheets>
-    <sheet name="results-1606074271" sheetId="1" r:id="rId1"/>
+    <sheet name="results-1606078946" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>graph</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>heuristic_time (ms)</t>
+  </si>
+  <si>
+    <t>cplex time (sec)</t>
+  </si>
+  <si>
+    <t>cplex time (ms)</t>
   </si>
   <si>
     <t>hamming6-2.clq</t>
@@ -918,15 +924,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -942,10 +948,16 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>32</v>
@@ -957,12 +969,42 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>29</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>32</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>16</v>
@@ -974,12 +1016,42 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>11</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>12</v>
@@ -991,12 +1063,42 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>138</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>65</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>110</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>75</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>24</v>
@@ -1008,12 +1110,42 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>120</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>67</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>96</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>92</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>55</v>
@@ -1025,12 +1157,42 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>17</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>316</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>15</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>365</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1042,12 +1204,42 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>6</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -1059,12 +1251,42 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>44</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>100</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>49</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>118</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>70</v>
@@ -1076,12 +1298,42 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>485</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>523</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>60</v>
@@ -1093,12 +1345,42 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>310</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>360</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>126</v>
@@ -1107,15 +1389,45 @@
         <v>126</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>2552</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1988</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>740</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1708</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>741</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1978</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>64</v>
@@ -1124,15 +1436,45 @@
         <v>64</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>1472</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>722</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>717</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>574</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>766</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>716</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>58</v>
@@ -1144,12 +1486,42 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>123</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>187</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>123</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>212</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>14</v>
@@ -1158,15 +1530,45 @@
         <v>14</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>1213</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>602</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>405</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>600</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>422</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>26</v>
@@ -1175,15 +1577,45 @@
         <v>26</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>617</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>414</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>621</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>462</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>18</v>
@@ -1195,12 +1627,42 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>27</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>111</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>28</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>128</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>34</v>
@@ -1212,12 +1674,42 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>7</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>122</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>7</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>131</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>11</v>
@@ -1229,12 +1721,42 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>45</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>52</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>68</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>60</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>12</v>
@@ -1246,12 +1768,42 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>141</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>60</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>141</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>76</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -1263,12 +1815,42 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>355</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>134</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>389</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>163</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>15</v>
@@ -1280,12 +1862,42 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>121</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>67</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>127</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>94</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>44</v>
@@ -1297,12 +1909,42 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>314</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>14</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>355</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>17</v>
@@ -1314,12 +1956,42 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>119</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>91</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>120</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>100</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>44</v>
@@ -1331,12 +2003,42 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>8</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>284</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>9</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>304</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>21</v>
@@ -1348,12 +2050,42 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>82</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>109</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>95</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>135</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -1365,12 +2097,42 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>256</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>225</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>282</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>269</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B27">
         <v>18</v>
@@ -1382,7 +2144,37 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>227</v>
+        <v>119</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>90</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>94</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>106</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>126</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>